<commit_message>
replaced HANA with SQL Server
</commit_message>
<xml_diff>
--- a/Tests/Manual Files/Customer_Priority.xlsx
+++ b/Tests/Manual Files/Customer_Priority.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">Customer</t>
   </si>
@@ -31,19 +31,10 @@
     <t xml:space="preserve">CUSTOMER1</t>
   </si>
   <si>
-    <t xml:space="preserve">PRIORITY1</t>
-  </si>
-  <si>
     <t xml:space="preserve">CUSTOMER2</t>
   </si>
   <si>
-    <t xml:space="preserve">PRIORITY2</t>
-  </si>
-  <si>
     <t xml:space="preserve">CUSTOMER3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRIORITY3</t>
   </si>
 </sst>
 </file>
@@ -58,6 +49,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -142,10 +134,10 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.61"/>
@@ -163,24 +155,24 @@
       <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>3</v>
+      <c r="B2" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>5</v>
+      <c r="B3" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>7</v>
+      <c r="B4" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>